<commit_message>
cooling and ventilation technologies added
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_EndUse.xlsx
+++ b/projects/test_building/input/ID_EndUse.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2204A9ED-6B8F-F549-8460-4C35E29F075D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7324EEF0-5724-1F41-AB67-9EA5D809DF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>id_end_use</t>
+  </si>
+  <si>
+    <t>ventilation</t>
   </si>
 </sst>
 </file>
@@ -93,8 +96,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_end_use"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
@@ -366,12 +369,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="261" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -413,6 +419,14 @@
       </c>
       <c r="B5" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some fine-tuning in window lifetime and availability of coal heating tech. Actions updated
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_EndUse.xlsx
+++ b/projects/test_building/input/ID_EndUse.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7324EEF0-5724-1F41-AB67-9EA5D809DF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,28 +24,28 @@
     <t>name</t>
   </si>
   <si>
-    <t>appliance electricity</t>
-  </si>
-  <si>
-    <t>domestic hot water</t>
-  </si>
-  <si>
-    <t>space heating</t>
-  </si>
-  <si>
-    <t>space cooling</t>
-  </si>
-  <si>
     <t>id_end_use</t>
   </si>
   <si>
-    <t>ventilation</t>
+    <t>Appliances</t>
+  </si>
+  <si>
+    <t>Space cooling</t>
+  </si>
+  <si>
+    <t>Space heating</t>
+  </si>
+  <si>
+    <t>Domestic hot water</t>
+  </si>
+  <si>
+    <t>Ventilation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,11 +95,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_end_use"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
+    <tableColumn id="1" name="id_end_use"/>
+    <tableColumn id="2" name="name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -368,60 +367,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="261" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>